<commit_message>
Added unicode and rich text reading.
</commit_message>
<xml_diff>
--- a/t/regression/xlsx_files/data01.xlsx
+++ b/t/regression/xlsx_files/data01.xlsx
@@ -10,8 +10,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Foo</t>
   </si>
@@ -34,12 +35,51 @@
   <si>
     <t>Moo</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This is a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rich</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>string</t>
+    </r>
+  </si>
+  <si>
+    <t>This is a unicode string €</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,6 +93,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -473,4 +520,32 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>